<commit_message>
origin destination distance for ajusted municipios
</commit_message>
<xml_diff>
--- a/data/adjusted_cetroid.xlsx
+++ b/data/adjusted_cetroid.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/transporte_hospitales/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanrosa/Desktop/r_projects/personal/transporte_hospitales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DCBED3-8D0F-F743-A50F-F0D694B86CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58173E2B-0A00-5C4D-900A-7CBC38674DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="520" windowWidth="28040" windowHeight="17440" xr2:uid="{D1A0C5F5-C027-3D4F-A51C-D11B3AC05CF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -173,9 +173,6 @@
     <t>San José De Las Matas</t>
   </si>
   <si>
-    <t>18.745353, -70.934893</t>
-  </si>
-  <si>
     <t>18.288210, -71.199149</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>new_location</t>
+  </si>
+  <si>
+    <t>18.745500, -70.935696</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -698,7 +698,7 @@
         <v>-70.765006372456</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>-71.209338535573707</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>-71.133772446333595</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -794,7 +794,7 @@
         <v>-71.153321465949503</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>-71.344416330952896</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
         <v>-71.317968827353297</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>-71.056913583021796</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -922,7 +922,7 @@
         <v>-71.628545405987495</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>-71.613356517168697</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>-71.518098305435302</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>-71.6477036135567</v>
       </c>
       <c r="J12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
         <v>-71.497642813617603</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>-70.215210556419393</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>-69.768176530112001</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
         <v>-70.034056263992994</v>
       </c>
       <c r="J16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
         <v>-70.132098064719102</v>
       </c>
       <c r="J17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>-69.883690306985301</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>-70.223930508731002</v>
       </c>
       <c r="J19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1274,7 +1274,7 @@
         <v>-70.021992646122698</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>-71.720509857583593</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
         <v>-71.640868434363298</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1370,7 +1370,7 @@
         <v>-71.670433335799004</v>
       </c>
       <c r="J23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1402,7 +1402,7 @@
         <v>-71.697448168929199</v>
       </c>
       <c r="J24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
         <v>-71.515376468302705</v>
       </c>
       <c r="J25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1466,7 +1466,7 @@
         <v>-71.025852550943995</v>
       </c>
       <c r="J26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>